<commit_message>
Updated sample forms and organization
</commit_message>
<xml_diff>
--- a/extras/sample-form-v2/Timed categories v2 sample form.xlsx
+++ b/extras/sample-form-v2/Timed categories v2 sample form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/Finalized/timed-categories/extras/sample-form-v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20D5BB1-169C-B243-AFA0-AF130FB04002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4499F0-8044-FE45-8969-70CFD8C6121B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2590,9 +2590,6 @@
     <t>metadata</t>
   </si>
   <si>
-    <t>If the choice selected is correct</t>
-  </si>
-  <si>
     <t>first_correct</t>
   </si>
   <si>
@@ -2722,6 +2719,9 @@
   </si>
   <si>
     <t>join(concat(linebreak(), linebreak()), ${result})</t>
+  </si>
+  <si>
+    <t>Choice value of the correct choice</t>
   </si>
 </sst>
 </file>
@@ -3639,8 +3639,9 @@
   <dxfs count="124">
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3697,6 +3698,141 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
@@ -3705,22 +3841,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3734,6 +3857,379 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99BCE7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE3E0CF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE7D480"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBB57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF2DBDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD44B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFBFB00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF9E004F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFE4E300"/>
@@ -3750,158 +4246,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3909,351 +4254,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99BCE7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDE8C6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE7D480"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFBB57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF2DBDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFD44B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFBFB00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF9E004F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEEB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4321,7 +4321,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFE3E0CF"/>
+          <bgColor rgb="FFEAEB74"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4329,6 +4329,14 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFDDE8C6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFBA005D"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4342,16 +4350,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFBA005D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <bgColor rgb="FFEAEB74"/>
+          <bgColor rgb="FFE3E0CF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4411,13 +4411,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6969"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4430,7 +4423,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFEEB400"/>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4444,21 +4444,60 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDCC97A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFE4E300"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF9900"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
+          <bgColor rgb="FF4685D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE1AAA9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4472,80 +4511,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF4685D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFDCC97A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFE4E300"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE1AAA9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FF9E004F"/>
@@ -4553,6 +4518,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4564,6 +4536,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -4576,7 +4555,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEEB400"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4584,6 +4577,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBBBB59"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5005,10 +5005,10 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N40" sqref="N40"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5205,7 +5205,7 @@
         <v>363</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>363</v>
@@ -5298,10 +5298,10 @@
         <v>362</v>
       </c>
       <c r="G14" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>414</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>415</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>381</v>
@@ -5345,7 +5345,7 @@
         <v>368</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -5924,7 +5924,7 @@
         <v>382</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>383</v>
@@ -5938,7 +5938,7 @@
         <v>120</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>262</v>
@@ -5985,7 +5985,7 @@
         <v>362</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O27" s="9" t="s">
         <v>362</v>
@@ -6157,12 +6157,15 @@
         <v>362</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>393</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>436</v>
       </c>
       <c r="N30" s="9" t="s">
         <v>394</v>
@@ -6173,10 +6176,10 @@
         <v>395</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>362</v>
@@ -6185,7 +6188,7 @@
         <v>362</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>362</v>
@@ -6243,9 +6246,6 @@
       <c r="B32" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>397</v>
-      </c>
       <c r="D32" s="11" t="s">
         <v>362</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>362</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O32" s="9" t="s">
         <v>362</v>
@@ -6312,10 +6312,10 @@
         <v>120</v>
       </c>
       <c r="B34" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="N34" s="9" t="s">
         <v>398</v>
-      </c>
-      <c r="N34" s="9" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
@@ -6323,10 +6323,10 @@
         <v>120</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="N35" s="9" t="s">
         <v>400</v>
-      </c>
-      <c r="N35" s="9" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
@@ -6334,10 +6334,10 @@
         <v>120</v>
       </c>
       <c r="B36" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="N36" s="9" t="s">
         <v>402</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="85" x14ac:dyDescent="0.2">
@@ -6345,11 +6345,11 @@
         <v>120</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>405</v>
-      </c>
       <c r="D37" s="11" t="s">
         <v>362</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>362</v>
       </c>
       <c r="N37" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O37" s="9" t="s">
         <v>362</v>
@@ -6424,10 +6424,10 @@
         <v>120</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
@@ -6435,10 +6435,10 @@
         <v>120</v>
       </c>
       <c r="B40" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="N40" s="9" t="s">
         <v>428</v>
-      </c>
-      <c r="N40" s="9" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
@@ -6446,10 +6446,10 @@
         <v>120</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
@@ -6457,10 +6457,10 @@
         <v>120</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44" spans="1:23" ht="119" x14ac:dyDescent="0.2">
@@ -6468,86 +6468,86 @@
         <v>40</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:W1048576">
-    <cfRule type="expression" dxfId="123" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="29" stopIfTrue="1">
+      <formula>$A1="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="2" stopIfTrue="1">
       <formula>$A1="file"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="56" stopIfTrue="1">
+      <formula>$A1="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="6" stopIfTrue="1">
       <formula>$A1="enumerator"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="55" stopIfTrue="1">
+      <formula>$A1="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="118" priority="10" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="53" stopIfTrue="1">
+      <formula>$A1="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="13" stopIfTrue="1">
       <formula>$A1="comments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="52" stopIfTrue="1">
+      <formula>$A1="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="114" priority="17" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="50" stopIfTrue="1">
+      <formula>$A1="integer"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="19" stopIfTrue="1">
       <formula>$A1="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="48" stopIfTrue="1">
+      <formula>$A1="decimal"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="110" priority="23" stopIfTrue="1">
       <formula>OR($A1="date", $A1="datetime", $A1="time")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="43" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="108" priority="25" stopIfTrue="1">
       <formula>OR($A1="calculate", $A1="calculate_here")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="36" stopIfTrue="1">
+      <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="106" priority="27" stopIfTrue="1">
       <formula>$A1="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="29" stopIfTrue="1">
-      <formula>$A1="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="113" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="33" stopIfTrue="1">
+      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="58" stopIfTrue="1">
+      <formula>$A1="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="31" stopIfTrue="1">
       <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="33" stopIfTrue="1">
-      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="36" stopIfTrue="1">
-      <formula>OR($A1="username", $A1="phonenumber", $A1="start", $A1="end", $A1="deviceid", $A1="subscriberid", $A1="simserial", $A1="caseid")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="43" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A1, 16)="select_multiple ", LEN($A1)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A1, 17)))), AND(LEFT($A1, 11)="select_one ", LEN($A1)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A1, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="109" priority="48" stopIfTrue="1">
-      <formula>$A1="decimal"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="50" stopIfTrue="1">
-      <formula>$A1="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="52" stopIfTrue="1">
-      <formula>$A1="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="53" stopIfTrue="1">
-      <formula>$A1="end repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="105" priority="55" stopIfTrue="1">
-      <formula>$A1="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="56" stopIfTrue="1">
-      <formula>$A1="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="58" stopIfTrue="1">
-      <formula>$A1="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 F1:F1048576">
-    <cfRule type="expression" dxfId="102" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="32" stopIfTrue="1">
+      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="101" priority="9" stopIfTrue="1">
       <formula>OR(AND(LEFT($A1, 14)="sensor_stream ", LEN($A1)&gt;14, NOT(ISNUMBER(SEARCH(" ", $A1, 15)))), AND(LEFT($A1, 17)="sensor_statistic ", LEN($A1)&gt;17, NOT(ISNUMBER(SEARCH(" ", $A1, 18)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="101" priority="32" stopIfTrue="1">
-      <formula>OR($A1="audio audit", $A1="text audit", $A1="speed violations count", $A1="speed violations list", $A1="speed violations audit")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 N1:N1048576">
@@ -6582,20 +6582,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="expression" dxfId="93" priority="1" stopIfTrue="1">
-      <formula>$A1="file"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="92" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="30" stopIfTrue="1">
+      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="26" stopIfTrue="1">
+      <formula>$A1="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="16" stopIfTrue="1">
       <formula>OR($A1="audio", $A1="video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="91" priority="26" stopIfTrue="1">
-      <formula>$A1="note"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="90" priority="28" stopIfTrue="1">
       <formula>$A1="barcode"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="30" stopIfTrue="1">
-      <formula>OR($A1="geopoint", $A1="geoshape", $A1="geotrace")</formula>
+    <cfRule type="expression" dxfId="89" priority="1" stopIfTrue="1">
+      <formula>$A1="file"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:D1048576 F1:F1048576">
@@ -6682,10 +6682,10 @@
         <v>31</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>407</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>408</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>362</v>
@@ -6696,13 +6696,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>409</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>410</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>411</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>362</v>
@@ -6710,13 +6710,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B6" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>412</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>413</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>362</v>
@@ -6779,7 +6779,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6815,14 +6815,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>418</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>419</v>
       </c>
       <c r="C2" s="16" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2312161534</v>
+        <v>2312161702</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>362</v>
@@ -10804,14 +10804,14 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:J6 L6:O6 Q6:S6">
-    <cfRule type="expression" dxfId="82" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="98" stopIfTrue="1">
+      <formula>$A6="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="95" stopIfTrue="1">
       <formula>$A6="begin repeat"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="96" stopIfTrue="1">
       <formula>$A6="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="98" stopIfTrue="1">
-      <formula>$A6="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:J6 Q6:S6">
@@ -10842,25 +10842,25 @@
     <cfRule type="expression" dxfId="71" priority="90" stopIfTrue="1">
       <formula>$A6="integer"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="93" stopIfTrue="1">
+      <formula>$A6="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="92" stopIfTrue="1">
       <formula>$A6="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
-      <formula>$A6="end repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:J6">
-    <cfRule type="expression" dxfId="68" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="73" stopIfTrue="1">
+      <formula>OR($A6="date", $A6="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="67" stopIfTrue="1">
       <formula>$A6="comments"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="69" stopIfTrue="1">
-      <formula>OR($A6="audio", $A6="video")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="66" priority="71" stopIfTrue="1">
       <formula>$A6="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="73" stopIfTrue="1">
-      <formula>OR($A6="date", $A6="datetime")</formula>
+    <cfRule type="expression" dxfId="65" priority="69" stopIfTrue="1">
+      <formula>OR($A6="audio", $A6="video")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6 H6">
@@ -10884,14 +10884,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6 H6">
-    <cfRule type="expression" dxfId="60" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="85" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="70" stopIfTrue="1">
       <formula>$A6="image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="72" stopIfTrue="1">
       <formula>OR($A6="date", $A6="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="85" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6 S6 L6">
@@ -10900,14 +10900,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6">
-    <cfRule type="expression" dxfId="56" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="78" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="55" priority="68" stopIfTrue="1">
       <formula>OR($A6="audio", $A6="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="76" stopIfTrue="1">
       <formula>$A6="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="54" priority="78" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="53" priority="80" stopIfTrue="1">
       <formula>$A6="geopoint"</formula>
@@ -10927,86 +10927,86 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="49" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="45" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="48" priority="46" stopIfTrue="1">
+      <formula>$A6="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="47" priority="47" stopIfTrue="1">
+      <formula>$A6="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="43" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="44" stopIfTrue="1">
+      <formula>$A6="geopoint"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="42" stopIfTrue="1">
+      <formula>$A6="note"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="41" stopIfTrue="1">
+      <formula>OR($A6="date", $A6="datetime")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="39" stopIfTrue="1">
       <formula>OR($A6="audio", $A6="video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="40" stopIfTrue="1">
       <formula>$A6="image"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="41" stopIfTrue="1">
-      <formula>OR($A6="date", $A6="datetime")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="42" stopIfTrue="1">
-      <formula>$A6="note"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="43" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="44" stopIfTrue="1">
-      <formula>$A6="geopoint"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="45" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="46" stopIfTrue="1">
-      <formula>$A6="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="47" stopIfTrue="1">
-      <formula>$A6="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="40" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="38" stopIfTrue="1">
+      <formula>$A6="begin group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="37" stopIfTrue="1">
+      <formula>$A6="end group"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="30" stopIfTrue="1">
       <formula>$A6="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="36" stopIfTrue="1">
+      <formula>$A6="begin repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="32" stopIfTrue="1">
       <formula>$A6="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="36" stopIfTrue="1">
-      <formula>$A6="begin repeat"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="37" stopIfTrue="1">
-      <formula>$A6="end group"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="38" stopIfTrue="1">
-      <formula>$A6="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:O6">
-    <cfRule type="expression" dxfId="35" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="34" stopIfTrue="1">
+      <formula>$A6="text"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="31" stopIfTrue="1">
       <formula>$A6="decimal"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="35" stopIfTrue="1">
+      <formula>$A6="end repeat"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="33" stopIfTrue="1">
       <formula>$A6="integer"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
-      <formula>$A6="text"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="35" stopIfTrue="1">
-      <formula>$A6="end repeat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:P6">
-    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
-      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="8" stopIfTrue="1">
+      <formula>$A6="geopoint"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
+      <formula>OR($A6="audio audit", $A6="text audit")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="6" stopIfTrue="1">
       <formula>$A6="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8" stopIfTrue="1">
-      <formula>$A6="geopoint"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9" stopIfTrue="1">
-      <formula>OR($A6="audio audit", $A6="text audit")</formula>
+    <cfRule type="expression" dxfId="27" priority="11" stopIfTrue="1">
+      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="26" priority="10" stopIfTrue="1">
       <formula>OR($A6="phonenumber", $A6="start", $A6="end", $A6="deviceid", $A6="subscriberid", $A6="simserial")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="11" stopIfTrue="1">
-      <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
+    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
+      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:AD6">
@@ -11047,14 +11047,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T6:AD6">
-    <cfRule type="expression" dxfId="13" priority="52" stopIfTrue="1">
-      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
+    <cfRule type="expression" dxfId="13" priority="54" stopIfTrue="1">
+      <formula>$A6="barcode"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="53" stopIfTrue="1">
       <formula>$A6="note"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="54" stopIfTrue="1">
-      <formula>$A6="barcode"</formula>
+    <cfRule type="expression" dxfId="11" priority="52" stopIfTrue="1">
+      <formula>OR($A6="calculate", $A6="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="10" priority="55" stopIfTrue="1">
       <formula>$A6="geopoint"</formula>
@@ -11062,8 +11062,8 @@
     <cfRule type="expression" dxfId="9" priority="56" stopIfTrue="1">
       <formula>OR($A6="audio audit", $A6="text audit")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="57" stopIfTrue="1">
-      <formula>OR($A6="phonenumber", $A6="start", $A6="end", $A6="deviceid", $A6="subscriberid", $A6="simserial")</formula>
+    <cfRule type="expression" dxfId="8" priority="65" stopIfTrue="1">
+      <formula>$A6="begin group"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="58" stopIfTrue="1">
       <formula>OR(AND(LEFT($A6, 16)="select_multiple ", LEN($A6)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A6, 17)))), AND(LEFT($A6, 11)="select_one ", LEN($A6)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A6, 12)))))</formula>
@@ -11086,8 +11086,8 @@
     <cfRule type="expression" dxfId="1" priority="64" stopIfTrue="1">
       <formula>$A6="end group"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="65" stopIfTrue="1">
-      <formula>$A6="begin group"</formula>
+    <cfRule type="expression" dxfId="0" priority="57" stopIfTrue="1">
+      <formula>OR($A6="phonenumber", $A6="start", $A6="end", $A6="deviceid", $A6="subscriberid", $A6="simserial")</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>